<commit_message>
Fixed RAD Test Cases and Data.  Added VLink Smoke Test Cases and Data.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042D74F9-BD81-4FC3-8951-39D585A6B48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{30AA0812-8EB4-4A43-B152-FA12F4B99A8C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="1590" windowWidth="23250" windowHeight="14730" xr2:uid="{466F649A-3E53-458C-A455-8A6BC3303076}"/>
+    <workbookView windowHeight="14730" windowWidth="23250" xWindow="1890" xr2:uid="{466F649A-3E53-458C-A455-8A6BC3303076}" yWindow="1590"/>
   </bookViews>
   <sheets>
-    <sheet name="NumberError" sheetId="1" r:id="rId1"/>
+    <sheet name="NumberError" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="117">
   <si>
     <t>Result</t>
   </si>
@@ -113,9 +113,6 @@
     <t>123456789</t>
   </si>
   <si>
-    <t>Thu Nov 03 15:36:10 EDT 2022</t>
-  </si>
-  <si>
     <t>Thu Nov 03 15:36:23 EDT 2022</t>
   </si>
   <si>
@@ -156,12 +153,247 @@
   </si>
   <si>
     <t>Thu Nov 03 15:38:41 EDT 2022</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:54:46 EDT 2022</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:55:33 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:55:45 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:55:55 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:56:05 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:56:15 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:56:25 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:56:35 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:56:44 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:56:54 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:57:03 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:57:13 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:57:23 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:57:33 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:57:42 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fri Nov 04 15:57:52 EDT 2022</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:08:59 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:09:08 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:09:18 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:09:28 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:09:37 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:09:48 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:09:57 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:10:08 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:10:18 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:10:27 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:10:38 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:10:47 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:10:57 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:11:07 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 14:11:17 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:40:01 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:40:11 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:40:20 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:40:30 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:40:40 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:40:51 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:41:01 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:41:12 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:41:21 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:41:31 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:41:41 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:41:52 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:42:02 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:42:12 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Jan 04 16:42:22 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:33:46 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:33:58 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:34:08 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:34:19 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:34:29 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:34:39 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:34:49 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:34:58 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:35:08 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:35:17 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:35:27 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:35:37 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:35:47 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:35:57 EST 2023</t>
+  </si>
+  <si>
+    <t>Fri Jan 06 18:36:06 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:50:24 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:50:33 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:50:42 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:50:52 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:51:02 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:51:11 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:51:21 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:51:31 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:51:41 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:51:51 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:52:01 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:52:11 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:52:21 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:52:30 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Jan 09 17:52:40 EST 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -204,20 +436,20 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -234,10 +466,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -272,7 +504,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -324,7 +556,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -435,21 +667,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -466,7 +698,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -518,30 +750,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6057E2E3-7C58-4120-B02D-BA3B396B9DA0}">
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6057E2E3-7C58-4120-B02D-BA3B396B9DA0}">
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C2" sqref="C2:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
-    <col min="2" max="2" width="27.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="2" collapsed="1"/>
-    <col min="4" max="4" width="20.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="55.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="27.85546875" collapsed="true"/>
+    <col min="3" max="3" style="2" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="35.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="16.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="55.28515625" collapsed="true"/>
+    <col min="8" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -572,9 +804,11 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>102</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
@@ -593,9 +827,11 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
@@ -614,9 +850,11 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
@@ -635,9 +873,11 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>105</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
@@ -656,9 +896,11 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -677,9 +919,11 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
@@ -698,9 +942,11 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>108</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
@@ -719,9 +965,11 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
@@ -740,9 +988,11 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>110</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
@@ -761,9 +1011,11 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>111</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
@@ -782,9 +1034,11 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>5</v>
       </c>
@@ -803,9 +1057,11 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>113</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>5</v>
       </c>
@@ -824,9 +1080,11 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>114</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>5</v>
       </c>
@@ -845,9 +1103,11 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>5</v>
       </c>
@@ -866,9 +1126,11 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>5</v>
       </c>
@@ -883,7 +1145,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Test Cases and data for VLink Card Not Accepted Error.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="147">
   <si>
     <t>Result</t>
   </si>
@@ -387,6 +387,96 @@
   </si>
   <si>
     <t>Mon Jan 09 17:52:40 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:05:01 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:05:10 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:05:20 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:05:30 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:05:40 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:05:49 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:05:59 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:06:09 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:06:19 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:06:28 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:06:39 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:06:48 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:06:58 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:07:08 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 12:07:18 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:44:06 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:44:15 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:44:26 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:44:36 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:44:46 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:44:56 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:45:07 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:45:16 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:45:26 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:45:36 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:45:46 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:45:56 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:46:06 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:46:16 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 08 16:46:26 EST 2023</t>
   </si>
 </sst>
 </file>
@@ -804,7 +894,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>39</v>
@@ -827,7 +917,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
@@ -850,7 +940,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>39</v>
@@ -873,7 +963,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>39</v>
@@ -896,7 +986,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>39</v>
@@ -919,7 +1009,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>39</v>
@@ -942,7 +1032,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>39</v>
@@ -965,7 +1055,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>39</v>
@@ -988,7 +1078,7 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>39</v>
@@ -1011,7 +1101,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
@@ -1034,7 +1124,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1057,7 +1147,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>39</v>
@@ -1080,7 +1170,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>39</v>
@@ -1103,7 +1193,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>145</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>39</v>
@@ -1126,7 +1216,7 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Made changes to RAD SaleAndUseUI Test Case.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="162">
   <si>
     <t>Result</t>
   </si>
@@ -477,6 +477,51 @@
   </si>
   <si>
     <t>Wed Feb 08 16:46:26 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:47:04 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:47:12 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:47:21 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:47:30 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:47:40 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:47:49 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:47:58 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:48:07 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:48:16 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:48:25 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:48:34 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:48:43 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:48:53 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:49:02 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Feb 15 12:49:10 EST 2023</t>
   </si>
 </sst>
 </file>
@@ -894,7 +939,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>39</v>
@@ -917,7 +962,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
@@ -940,7 +985,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>39</v>
@@ -963,7 +1008,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>39</v>
@@ -986,7 +1031,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>39</v>
@@ -1009,7 +1054,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>39</v>
@@ -1032,7 +1077,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>39</v>
@@ -1055,7 +1100,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>39</v>
@@ -1078,7 +1123,7 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>39</v>
@@ -1101,7 +1146,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
@@ -1124,7 +1169,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1147,7 +1192,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>39</v>
@@ -1170,7 +1215,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>39</v>
@@ -1193,7 +1238,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>39</v>
@@ -1216,7 +1261,7 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
No Major changes.  Committed thru desktop for laptop.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="177">
   <si>
     <t>Result</t>
   </si>
@@ -522,6 +522,51 @@
   </si>
   <si>
     <t>Wed Feb 15 12:49:10 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:14:13 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:14:22 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:14:31 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:14:40 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:14:49 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:14:58 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:15:08 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:15:17 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:15:26 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:15:35 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:15:45 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:15:54 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:16:03 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:16:12 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Feb 16 12:16:21 EST 2023</t>
   </si>
 </sst>
 </file>
@@ -939,7 +984,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>39</v>
@@ -962,7 +1007,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
@@ -985,7 +1030,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>39</v>
@@ -1008,7 +1053,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>39</v>
@@ -1031,7 +1076,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>39</v>
@@ -1054,7 +1099,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>39</v>
@@ -1077,7 +1122,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>39</v>
@@ -1100,7 +1145,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>39</v>
@@ -1123,7 +1168,7 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>39</v>
@@ -1146,7 +1191,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
@@ -1169,7 +1214,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1192,7 +1237,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>39</v>
@@ -1215,7 +1260,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>39</v>
@@ -1238,7 +1283,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>39</v>
@@ -1261,7 +1306,7 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Added Gateway Production and Upgrade Live Processors Test Cases and Test Suites.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="192">
   <si>
     <t>Result</t>
   </si>
@@ -567,6 +567,51 @@
   </si>
   <si>
     <t>Thu Feb 16 12:16:21 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:57:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:57:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:57:58 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:58:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:58:16 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:58:25 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:58:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:58:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:58:51 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:58:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:59:08 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:59:17 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:59:26 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:59:34 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Jul 11 12:59:43 EDT 2023</t>
   </si>
 </sst>
 </file>
@@ -984,7 +1029,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>39</v>
@@ -1007,7 +1052,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
@@ -1030,7 +1075,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>39</v>
@@ -1053,7 +1098,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>39</v>
@@ -1076,7 +1121,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>39</v>
@@ -1099,7 +1144,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>39</v>
@@ -1122,7 +1167,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>39</v>
@@ -1145,7 +1190,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>39</v>
@@ -1168,7 +1213,7 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>39</v>
@@ -1191,7 +1236,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
@@ -1214,7 +1259,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1237,7 +1282,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>39</v>
@@ -1260,7 +1305,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>39</v>
@@ -1283,7 +1328,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>39</v>
@@ -1306,7 +1351,7 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Added Test Cases for RAD Updates for August 30, Phase 2.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="252">
   <si>
     <t>Result</t>
   </si>
@@ -612,6 +612,186 @@
   </si>
   <si>
     <t>Tue Jul 11 12:59:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:48:48 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:48:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:49:05 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:49:14 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:49:23 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:49:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:49:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:49:49 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:49:58 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:50:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:50:16 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:50:25 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:50:34 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:50:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 10:50:52 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:12:10 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:12:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:12:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:12:36 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:12:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:12:54 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:13:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:13:11 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:13:20 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:13:29 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:13:38 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:13:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:13:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:14:04 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Jul 16 12:14:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:21:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:21:58 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:22:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:22:16 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:22:25 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:22:34 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:22:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:22:52 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:23:01 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:23:10 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:23:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:23:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:23:36 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:23:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 19:23:54 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:14:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:14:15 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:14:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:14:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:14:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:14:52 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:15:00 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:15:09 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:15:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:15:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:15:36 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:15:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:15:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:16:04 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Jul 17 21:16:13 EDT 2023</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1209,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>39</v>
@@ -1052,7 +1232,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>238</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
@@ -1075,7 +1255,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>39</v>
@@ -1098,7 +1278,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>39</v>
@@ -1121,7 +1301,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>241</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>39</v>
@@ -1144,7 +1324,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>242</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>39</v>
@@ -1167,7 +1347,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>183</v>
+        <v>243</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>39</v>
@@ -1190,7 +1370,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>244</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>39</v>
@@ -1213,7 +1393,7 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>185</v>
+        <v>245</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>39</v>
@@ -1236,7 +1416,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>186</v>
+        <v>246</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
@@ -1259,7 +1439,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>247</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1282,7 +1462,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>188</v>
+        <v>248</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>39</v>
@@ -1305,7 +1485,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>189</v>
+        <v>249</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>39</v>
@@ -1328,7 +1508,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>190</v>
+        <v>250</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>39</v>
@@ -1351,7 +1531,7 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>191</v>
+        <v>251</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Fixed and Added RAD Negative Test Cases.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04550FD0-FCC4-4A41-AF22-50C9787C9935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{522DE480-86C3-4D9E-848E-7A99F091A816}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{466F649A-3E53-458C-A455-8A6BC3303076}"/>
+    <workbookView windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{466F649A-3E53-458C-A455-8A6BC3303076}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="NumberError" sheetId="1" r:id="rId1"/>
+    <sheet name="NumberError" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="44">
   <si>
     <t>Result</t>
   </si>
@@ -53,27 +53,12 @@
     <t>TaxTypeEL</t>
   </si>
   <si>
-    <t>Existing Liability</t>
-  </si>
-  <si>
-    <t>Bay Restoration Fund Tax</t>
-  </si>
-  <si>
-    <t>CORP Tax</t>
-  </si>
-  <si>
     <t>Fiduciary Tax</t>
   </si>
   <si>
-    <t>Personal Tax</t>
-  </si>
-  <si>
     <t>Sales &amp; Use Tax</t>
   </si>
   <si>
-    <t>Tire Fee Tax</t>
-  </si>
-  <si>
     <t>Withholding Tax</t>
   </si>
   <si>
@@ -98,73 +83,98 @@
     <t>Notice number length has to be 13 numeric characters</t>
   </si>
   <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Existing Liability w/Notice Number</t>
+  </si>
+  <si>
+    <t>Bay Restoration Fee</t>
+  </si>
+  <si>
+    <t>Corporate Income Tax</t>
+  </si>
+  <si>
+    <t>Personal Income Tax</t>
+  </si>
+  <si>
+    <t>PTE Non-Electing Non-S Corp</t>
+  </si>
+  <si>
+    <t>PTE Non-Electing S Corp</t>
+  </si>
+  <si>
+    <t>Tire Recycling Fee</t>
+  </si>
+  <si>
+    <t>PTE Tax Electing Non-S Corp</t>
+  </si>
+  <si>
+    <t>PTE Tax Electing S Corp</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:14:07 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:14:15 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:14:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:14:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:14:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:14:52 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:15:09 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:15:18 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:15:27 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:15:36 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:15:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:15:55 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:16:04 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 21:16:13 EDT 2023</t>
-  </si>
-  <si>
-    <t>PTE (510 LLC) Tax</t>
-  </si>
-  <si>
-    <t>PTE (510 SCorp) Tax</t>
-  </si>
-  <si>
-    <t>PTEE (511 LLC) Tax</t>
-  </si>
-  <si>
-    <t>PTEE (511 SCorp) Tax</t>
+    <t>Sun Sep 03 16:19:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:19:30 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:19:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:19:51 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:20:01 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:20:11 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:20:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:20:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:20:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:20:51 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:21:01 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:21:11 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:21:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:21:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:21:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sun Sep 03 16:21:51 EDT 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,20 +217,20 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -237,10 +247,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -275,7 +285,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -327,7 +337,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -438,21 +448,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -469,7 +479,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -521,30 +531,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6057E2E3-7C58-4120-B02D-BA3B396B9DA0}">
-  <dimension ref="A1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6057E2E3-7C58-4120-B02D-BA3B396B9DA0}">
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E17"/>
+      <selection activeCell="A2" sqref="A2:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
-    <col min="2" max="2" width="27.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" style="2" collapsed="1"/>
-    <col min="4" max="4" width="20.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="55.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="27.85546875" collapsed="true"/>
+    <col min="3" max="3" style="2" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="48.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="42.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="16.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="55.28515625" collapsed="true"/>
+    <col min="8" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -564,375 +574,383 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17"/>
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
       <c r="C17" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updated RAD Test Cases.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{522DE480-86C3-4D9E-848E-7A99F091A816}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{52C79347-470B-4D6A-B8EA-833F892A5823}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{466F649A-3E53-458C-A455-8A6BC3303076}" yWindow="-120"/>
+    <workbookView windowHeight="10740" windowWidth="18915" xWindow="7830" xr2:uid="{466F649A-3E53-458C-A455-8A6BC3303076}" yWindow="3435"/>
   </bookViews>
   <sheets>
     <sheet name="NumberError" r:id="rId1" sheetId="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="93">
   <si>
     <t>Result</t>
   </si>
@@ -53,9 +53,114 @@
     <t>TaxTypeEL</t>
   </si>
   <si>
+    <t>NotiInvoNumber</t>
+  </si>
+  <si>
+    <t>12345678901</t>
+  </si>
+  <si>
+    <t>123456789012</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>Invoice number length has to be 10 or 13 numeric characters</t>
+  </si>
+  <si>
+    <t>Notice number length has to be 13 numeric characters</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Existing Liability w/Notice Number</t>
+  </si>
+  <si>
+    <t>Bay Restoration Fee</t>
+  </si>
+  <si>
+    <t>PTE Non-Electing Non-S Corp</t>
+  </si>
+  <si>
+    <t>PTE Non-Electing S Corp</t>
+  </si>
+  <si>
+    <t>Tire Recycling Fee</t>
+  </si>
+  <si>
+    <t>PTE Tax Electing Non-S Corp</t>
+  </si>
+  <si>
+    <t>PTE Tax Electing S Corp</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:20:12 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:20:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:20:30 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:20:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:20:49 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:20:57 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:21:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:21:16 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:21:26 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:21:36 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:21:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:21:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:22:04 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:22:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:22:23 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 07 12:22:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Corporate Income Tax</t>
+  </si>
+  <si>
     <t>Fiduciary Tax</t>
   </si>
   <si>
+    <t>Personal Income Tax</t>
+  </si>
+  <si>
     <t>Sales &amp; Use Tax</t>
   </si>
   <si>
@@ -65,109 +170,151 @@
     <t>Alcohol Tax</t>
   </si>
   <si>
-    <t>NotiInvoNumber</t>
-  </si>
-  <si>
-    <t>12345678901</t>
-  </si>
-  <si>
-    <t>123456789012</t>
-  </si>
-  <si>
-    <t>ErrorMessage</t>
-  </si>
-  <si>
-    <t>Invoice number length has to be 10 or 13 numeric characters</t>
-  </si>
-  <si>
-    <t>Notice number length has to be 13 numeric characters</t>
-  </si>
-  <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Existing Liability w/Notice Number</t>
-  </si>
-  <si>
-    <t>Bay Restoration Fee</t>
-  </si>
-  <si>
-    <t>Corporate Income Tax</t>
-  </si>
-  <si>
-    <t>Personal Income Tax</t>
-  </si>
-  <si>
-    <t>PTE Non-Electing Non-S Corp</t>
-  </si>
-  <si>
-    <t>PTE Non-Electing S Corp</t>
-  </si>
-  <si>
-    <t>Tire Recycling Fee</t>
-  </si>
-  <si>
-    <t>PTE Tax Electing Non-S Corp</t>
-  </si>
-  <si>
-    <t>PTE Tax Electing S Corp</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:19:18 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:19:30 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:19:40 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:19:51 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:20:01 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:20:11 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:20:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:20:31 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:20:41 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:20:51 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:21:01 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:21:11 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:21:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:21:31 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:21:41 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Sep 03 16:21:51 EDT 2023</t>
+    <t>Fri Sep 08 12:30:39 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:30:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:31:00 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:31:10 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:31:20 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:31:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:31:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:31:51 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:32:01 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:32:11 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:32:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:32:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:32:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:32:51 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:33:01 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 12:33:12 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:22:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:22:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:22:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:22:35 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:22:46 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:22:57 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:23:08 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:23:19 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:23:30 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:23:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:23:52 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:24:03 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:24:14 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:24:25 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:24:36 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 16:24:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 17:59:57 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:00:08 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:00:19 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:00:30 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:00:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:00:52 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:01:03 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:01:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:01:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:01:35 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:01:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:01:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:02:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:02:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:02:29 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 08 18:02:39 EDT 2023</t>
   </si>
 </sst>
 </file>
@@ -542,7 +689,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,378 +721,378 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added RAD BeforePayments Test Cases and Test Data.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="141">
   <si>
     <t>Result</t>
   </si>
@@ -315,6 +315,150 @@
   </si>
   <si>
     <t>Fri Sep 08 18:02:39 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:43:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:44:05 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:44:15 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:44:26 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:44:35 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:44:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:44:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:45:05 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:45:15 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:45:25 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:45:37 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:45:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:45:57 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:46:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:46:17 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Sep 09 20:46:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:55:16 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:55:26 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:55:36 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:55:46 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:55:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:56:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:56:17 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:56:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:56:37 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:56:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:56:57 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:57:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:57:17 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:57:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:57:37 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 12:57:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:53:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:53:54 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:54:04 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:54:14 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:54:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:54:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:54:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:54:53 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:55:03 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:55:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:55:22 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:55:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:55:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:55:52 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:56:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Mon Sep 11 13:56:12 EDT 2023</t>
   </si>
 </sst>
 </file>
@@ -732,7 +876,7 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
@@ -755,7 +899,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -778,7 +922,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -801,7 +945,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -824,7 +968,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -847,7 +991,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
@@ -870,7 +1014,7 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -893,7 +1037,7 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>132</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -916,7 +1060,7 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -939,7 +1083,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
@@ -962,7 +1106,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
@@ -985,7 +1129,7 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>136</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
@@ -1008,7 +1152,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>137</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -1031,7 +1175,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>138</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
@@ -1054,7 +1198,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
@@ -1077,7 +1221,7 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Updated RAD Notice Number Error Message.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FF28F5-A774-4574-BF9A-B099397BF1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7684F7CF-1EDB-4F65-B9CB-2D0318F01326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{466F649A-3E53-458C-A455-8A6BC3303076}"/>
+    <workbookView xWindow="3525" yWindow="1650" windowWidth="18810" windowHeight="14565" xr2:uid="{466F649A-3E53-458C-A455-8A6BC3303076}"/>
   </bookViews>
   <sheets>
     <sheet name="NumberError" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="59">
   <si>
     <t>Result</t>
   </si>
@@ -65,12 +65,6 @@
     <t>ErrorMessage</t>
   </si>
   <si>
-    <t>Invoice number length has to be 10 or 13 numeric characters</t>
-  </si>
-  <si>
-    <t>Notice number length has to be 13 numeric characters</t>
-  </si>
-  <si>
     <t>123456789</t>
   </si>
   <si>
@@ -119,54 +113,6 @@
     <t>Alcohol Tax</t>
   </si>
   <si>
-    <t>Thu Dec 07 21:34:43 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:34:52 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:35:01 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:35:10 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:35:19 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:35:29 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:35:38 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:35:47 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:35:56 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:36:05 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:36:14 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:36:23 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:36:32 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:36:41 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:36:50 EST 2023</t>
-  </si>
-  <si>
-    <t>Thu Dec 07 21:36:59 EST 2023</t>
-  </si>
-  <si>
     <t>0000000000000</t>
   </si>
   <si>
@@ -177,6 +123,96 @@
   </si>
   <si>
     <t>Invoice Number must be 10 or 13 digits in length, with a value greater than zero</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:46:49 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:46:59 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:47:09 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:47:18 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:47:28 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:47:37 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:47:47 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:47:56 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:48:06 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:48:16 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:48:25 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:48:34 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:48:44 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:48:54 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:49:04 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:49:14 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:49:24 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:49:35 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:49:44 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:49:54 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:50:03 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:50:13 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:50:22 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:50:32 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:50:42 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:50:51 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:51:01 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:51:10 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:51:20 EST 2023</t>
+  </si>
+  <si>
+    <t>Wed Dec 20 12:51:29 EST 2023</t>
   </si>
 </sst>
 </file>
@@ -549,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6057E2E3-7C58-4120-B02D-BA3B396B9DA0}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,636 +626,692 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="F21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="F25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="F27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="F30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="F31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="G31" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to Phase 3 RAD Non-UI Test Cases and Data
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7684F7CF-1EDB-4F65-B9CB-2D0318F01326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A36DC4-16A4-4D51-BCA4-4B212B5FB9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="1650" windowWidth="18810" windowHeight="14565" xr2:uid="{466F649A-3E53-458C-A455-8A6BC3303076}"/>
+    <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="17640" xr2:uid="{466F649A-3E53-458C-A455-8A6BC3303076}"/>
   </bookViews>
   <sheets>
     <sheet name="NumberError" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="67">
   <si>
     <t>Result</t>
   </si>
@@ -213,6 +213,30 @@
   </si>
   <si>
     <t>Wed Dec 20 12:51:29 EST 2023</t>
+  </si>
+  <si>
+    <t>Admissions and Amusement Tax</t>
+  </si>
+  <si>
+    <t>Estate Tax</t>
+  </si>
+  <si>
+    <t>Motor Fuel Tax</t>
+  </si>
+  <si>
+    <t>Slots License Fee</t>
+  </si>
+  <si>
+    <t>Tobacco Tax</t>
+  </si>
+  <si>
+    <t>Transportation Network Services</t>
+  </si>
+  <si>
+    <t>Unclaimed Property</t>
+  </si>
+  <si>
+    <t>IFTA Tax</t>
   </si>
 </sst>
 </file>
@@ -583,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6057E2E3-7C58-4120-B02D-BA3B396B9DA0}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,9 +619,9 @@
     <col min="2" max="2" width="27.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.140625" style="2" collapsed="1"/>
     <col min="4" max="4" width="48.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="42.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="71.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="53.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="80.5703125" style="2" customWidth="1" collapsed="1"/>
     <col min="8" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1311,6 +1335,278 @@
         <v>25</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated RAD Test Cases and Test Data for Existing Liability.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C732893E-1BA4-426A-AE00-8A780CCB884B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81C39F4-074C-44BA-8EDD-5ACF17B0DF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1965" yWindow="1155" windowWidth="24525" windowHeight="14010" xr2:uid="{466F649A-3E53-458C-A455-8A6BC3303076}"/>
   </bookViews>
@@ -673,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83D66D2-4D2B-4A65-94BC-7BBA002436C7}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C61"/>
+    <sheetView tabSelected="1" topLeftCell="C36" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Latest Code for RAD Production Release Nov 08 2024
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="261">
   <si>
     <t>Result</t>
   </si>
@@ -649,6 +649,177 @@
   </si>
   <si>
     <t>Thu Nov 07 20:05:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:42:17 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:42:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:42:39 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:42:48 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:42:58 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:43:07 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:43:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:43:26 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:43:36 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:43:48 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:43:58 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:44:07 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:44:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:44:25 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:44:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:44:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:44:56 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:45:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:45:15 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:45:24 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:45:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:45:46 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:45:55 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:46:05 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:46:14 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:46:24 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:46:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:46:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:46:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:47:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:47:13 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:47:23 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:47:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:47:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:47:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:48:03 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:48:13 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:48:22 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:48:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:48:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:48:54 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:49:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:49:15 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:49:25 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:49:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:49:50 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:49:59 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:50:08 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:50:17 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:50:28 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:50:38 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:50:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:50:57 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:51:07 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:51:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:51:26 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Nov 12 17:51:35 EST 2024</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1237,7 @@
         <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>204</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -1089,7 +1260,7 @@
         <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>205</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -1112,7 +1283,7 @@
         <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>206</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
@@ -1135,7 +1306,7 @@
         <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>207</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -1158,7 +1329,7 @@
         <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>208</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -1181,7 +1352,7 @@
         <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>209</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
@@ -1204,7 +1375,7 @@
         <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>210</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
@@ -1227,7 +1398,7 @@
         <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -1250,7 +1421,7 @@
         <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -1273,7 +1444,7 @@
         <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>213</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>10</v>
@@ -1296,7 +1467,7 @@
         <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>214</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>10</v>
@@ -1319,7 +1490,7 @@
         <v>84</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>215</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>10</v>
@@ -1342,7 +1513,7 @@
         <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>10</v>
@@ -1365,7 +1536,7 @@
         <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>217</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>10</v>
@@ -1388,7 +1559,7 @@
         <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>218</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>10</v>
@@ -1411,7 +1582,7 @@
         <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
+        <v>219</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>10</v>
@@ -1434,7 +1605,7 @@
         <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>220</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>10</v>
@@ -1457,7 +1628,7 @@
         <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>221</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>10</v>
@@ -1480,7 +1651,7 @@
         <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
+        <v>222</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
@@ -1503,7 +1674,7 @@
         <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>166</v>
+        <v>223</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>10</v>
@@ -1526,7 +1697,7 @@
         <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>167</v>
+        <v>224</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>10</v>
@@ -1549,7 +1720,7 @@
         <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>168</v>
+        <v>225</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>10</v>
@@ -1572,7 +1743,7 @@
         <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>169</v>
+        <v>226</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>10</v>
@@ -1595,7 +1766,7 @@
         <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>170</v>
+        <v>227</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>10</v>
@@ -1618,7 +1789,7 @@
         <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>171</v>
+        <v>228</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>10</v>
@@ -1641,7 +1812,7 @@
         <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>172</v>
+        <v>229</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>10</v>
@@ -1664,7 +1835,7 @@
         <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>173</v>
+        <v>230</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>10</v>
@@ -1687,7 +1858,7 @@
         <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>174</v>
+        <v>231</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>10</v>
@@ -1710,7 +1881,7 @@
         <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>175</v>
+        <v>232</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>10</v>
@@ -1733,7 +1904,7 @@
         <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>176</v>
+        <v>233</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>10</v>
@@ -1756,7 +1927,7 @@
         <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>177</v>
+        <v>234</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>10</v>
@@ -1779,7 +1950,7 @@
         <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>178</v>
+        <v>235</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>10</v>
@@ -1802,7 +1973,7 @@
         <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>179</v>
+        <v>236</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>10</v>
@@ -1825,7 +1996,7 @@
         <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>180</v>
+        <v>237</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>10</v>
@@ -1848,7 +2019,7 @@
         <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>10</v>
@@ -1871,7 +2042,7 @@
         <v>84</v>
       </c>
       <c r="B37" t="s">
-        <v>182</v>
+        <v>239</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>10</v>
@@ -1894,7 +2065,7 @@
         <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>183</v>
+        <v>240</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>10</v>
@@ -1917,7 +2088,7 @@
         <v>84</v>
       </c>
       <c r="B39" t="s">
-        <v>184</v>
+        <v>241</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>10</v>
@@ -1940,7 +2111,7 @@
         <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>185</v>
+        <v>242</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>10</v>
@@ -2032,7 +2203,7 @@
         <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>186</v>
+        <v>243</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>10</v>
@@ -2055,7 +2226,7 @@
         <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>244</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>10</v>
@@ -2078,7 +2249,7 @@
         <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>188</v>
+        <v>245</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>10</v>
@@ -2101,7 +2272,7 @@
         <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>189</v>
+        <v>246</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>10</v>
@@ -2124,7 +2295,7 @@
         <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>190</v>
+        <v>247</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>10</v>
@@ -2147,7 +2318,7 @@
         <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>191</v>
+        <v>248</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>10</v>
@@ -2170,7 +2341,7 @@
         <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>192</v>
+        <v>249</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>10</v>
@@ -2193,7 +2364,7 @@
         <v>84</v>
       </c>
       <c r="B51" t="s">
-        <v>193</v>
+        <v>250</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>10</v>
@@ -2216,7 +2387,7 @@
         <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>194</v>
+        <v>251</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>10</v>
@@ -2239,7 +2410,7 @@
         <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>195</v>
+        <v>252</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>10</v>
@@ -2262,7 +2433,7 @@
         <v>84</v>
       </c>
       <c r="B54" t="s">
-        <v>196</v>
+        <v>253</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>10</v>
@@ -2285,7 +2456,7 @@
         <v>84</v>
       </c>
       <c r="B55" t="s">
-        <v>197</v>
+        <v>254</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>10</v>
@@ -2308,7 +2479,7 @@
         <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>198</v>
+        <v>255</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>10</v>
@@ -2331,7 +2502,7 @@
         <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>10</v>
@@ -2354,7 +2525,7 @@
         <v>84</v>
       </c>
       <c r="B58" t="s">
-        <v>200</v>
+        <v>257</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>10</v>
@@ -2377,7 +2548,7 @@
         <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>201</v>
+        <v>258</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>10</v>
@@ -2400,7 +2571,7 @@
         <v>84</v>
       </c>
       <c r="B60" t="s">
-        <v>202</v>
+        <v>259</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>10</v>
@@ -2423,7 +2594,7 @@
         <v>84</v>
       </c>
       <c r="B61" t="s">
-        <v>203</v>
+        <v>260</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Updated RAD Summary test cases
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EL-NumberValidation.xlsx
+++ b/KatalonData/RADTestData/EL-NumberValidation.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="280">
   <si>
     <t>Result</t>
   </si>
@@ -679,6 +679,204 @@
   </si>
   <si>
     <t>Tue Feb 11 20:07:27 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:38:26 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:38:37 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:38:47 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:38:58 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:39:08 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:39:19 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:39:29 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:39:40 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:39:51 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:40:01 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:40:11 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:40:22 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:40:32 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:40:42 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:40:52 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:41:02 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:41:12 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:41:23 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:41:34 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:41:44 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:41:55 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:42:05 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:42:15 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:42:25 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:42:35 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:42:45 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:42:55 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:43:05 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:43:15 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:43:26 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:43:36 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:43:49 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:43:58 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:44:10 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:44:22 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:44:32 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:44:42 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:44:52 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:45:02 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:45:12 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:45:24 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:45:33 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:45:43 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:45:53 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:46:03 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:46:14 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:46:23 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:46:33 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:46:43 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:46:53 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:47:03 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:47:13 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:47:23 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:47:34 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:47:44 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:47:54 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:48:05 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:48:15 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:48:26 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:48:40 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:48:50 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:48:59 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:49:09 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:49:20 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:49:30 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Feb 24 22:49:40 EST 2025</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1294,7 @@
         <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>214</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -1119,7 +1317,7 @@
         <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>215</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -1142,7 +1340,7 @@
         <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>216</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
@@ -1165,7 +1363,7 @@
         <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>217</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -1188,7 +1386,7 @@
         <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>218</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -1211,7 +1409,7 @@
         <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>219</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
@@ -1234,7 +1432,7 @@
         <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>220</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
@@ -1257,7 +1455,7 @@
         <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>221</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -1280,7 +1478,7 @@
         <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>222</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -1303,7 +1501,7 @@
         <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>223</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>10</v>
@@ -1326,7 +1524,7 @@
         <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>224</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>10</v>
@@ -1349,7 +1547,7 @@
         <v>84</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>225</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>10</v>
@@ -1372,7 +1570,7 @@
         <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>226</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>10</v>
@@ -1395,7 +1593,7 @@
         <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>227</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>10</v>
@@ -1418,7 +1616,7 @@
         <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>228</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>10</v>
@@ -1441,7 +1639,7 @@
         <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>229</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>10</v>
@@ -1464,7 +1662,7 @@
         <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>230</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>10</v>
@@ -1487,7 +1685,7 @@
         <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>165</v>
+        <v>231</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>10</v>
@@ -1510,7 +1708,7 @@
         <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>232</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
@@ -1533,7 +1731,7 @@
         <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>167</v>
+        <v>233</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>10</v>
@@ -1556,7 +1754,7 @@
         <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>168</v>
+        <v>234</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>10</v>
@@ -1579,7 +1777,7 @@
         <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>235</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>10</v>
@@ -1602,7 +1800,7 @@
         <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>170</v>
+        <v>236</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>10</v>
@@ -1625,7 +1823,7 @@
         <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>171</v>
+        <v>237</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>10</v>
@@ -1648,7 +1846,7 @@
         <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>172</v>
+        <v>238</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>10</v>
@@ -1671,7 +1869,7 @@
         <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>239</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>10</v>
@@ -1694,7 +1892,7 @@
         <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>240</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>10</v>
@@ -1717,7 +1915,7 @@
         <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>175</v>
+        <v>241</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>10</v>
@@ -1740,7 +1938,7 @@
         <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>10</v>
@@ -1763,7 +1961,7 @@
         <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>177</v>
+        <v>243</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>10</v>
@@ -1786,7 +1984,7 @@
         <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>178</v>
+        <v>244</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>10</v>
@@ -1809,7 +2007,7 @@
         <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>179</v>
+        <v>245</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>10</v>
@@ -1832,7 +2030,7 @@
         <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>180</v>
+        <v>246</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>10</v>
@@ -1855,7 +2053,7 @@
         <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>181</v>
+        <v>247</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>10</v>
@@ -1878,7 +2076,7 @@
         <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>182</v>
+        <v>248</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>10</v>
@@ -1901,7 +2099,7 @@
         <v>84</v>
       </c>
       <c r="B37" t="s">
-        <v>183</v>
+        <v>249</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>10</v>
@@ -1924,7 +2122,7 @@
         <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>184</v>
+        <v>250</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>10</v>
@@ -1947,7 +2145,7 @@
         <v>84</v>
       </c>
       <c r="B39" t="s">
-        <v>185</v>
+        <v>251</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>10</v>
@@ -1970,7 +2168,7 @@
         <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>186</v>
+        <v>252</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>10</v>
@@ -1993,7 +2191,7 @@
         <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>187</v>
+        <v>253</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>10</v>
@@ -2016,7 +2214,7 @@
         <v>84</v>
       </c>
       <c r="B42" t="s">
-        <v>188</v>
+        <v>254</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>10</v>
@@ -2039,7 +2237,7 @@
         <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>189</v>
+        <v>255</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>10</v>
@@ -2062,7 +2260,7 @@
         <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>190</v>
+        <v>256</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>10</v>
@@ -2085,7 +2283,7 @@
         <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>191</v>
+        <v>257</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>10</v>
@@ -2108,7 +2306,7 @@
         <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>192</v>
+        <v>258</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>10</v>
@@ -2131,7 +2329,7 @@
         <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>193</v>
+        <v>259</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>10</v>
@@ -2154,7 +2352,7 @@
         <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>194</v>
+        <v>260</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>10</v>
@@ -2177,7 +2375,7 @@
         <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>195</v>
+        <v>261</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>10</v>
@@ -2200,7 +2398,7 @@
         <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>10</v>
@@ -2223,7 +2421,7 @@
         <v>84</v>
       </c>
       <c r="B51" t="s">
-        <v>197</v>
+        <v>263</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>10</v>
@@ -2246,7 +2444,7 @@
         <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>198</v>
+        <v>264</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>10</v>
@@ -2269,7 +2467,7 @@
         <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>199</v>
+        <v>265</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>10</v>
@@ -2292,7 +2490,7 @@
         <v>84</v>
       </c>
       <c r="B54" t="s">
-        <v>200</v>
+        <v>266</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>10</v>
@@ -2315,7 +2513,7 @@
         <v>84</v>
       </c>
       <c r="B55" t="s">
-        <v>201</v>
+        <v>267</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>10</v>
@@ -2338,7 +2536,7 @@
         <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>202</v>
+        <v>268</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>10</v>
@@ -2361,7 +2559,7 @@
         <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>203</v>
+        <v>269</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>10</v>
@@ -2384,7 +2582,7 @@
         <v>84</v>
       </c>
       <c r="B58" t="s">
-        <v>204</v>
+        <v>270</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>10</v>
@@ -2407,7 +2605,7 @@
         <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>205</v>
+        <v>271</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>10</v>
@@ -2430,7 +2628,7 @@
         <v>84</v>
       </c>
       <c r="B60" t="s">
-        <v>206</v>
+        <v>272</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>10</v>
@@ -2453,7 +2651,7 @@
         <v>84</v>
       </c>
       <c r="B61" t="s">
-        <v>207</v>
+        <v>273</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>10</v>
@@ -2476,7 +2674,7 @@
         <v>84</v>
       </c>
       <c r="B62" t="s">
-        <v>208</v>
+        <v>274</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>10</v>
@@ -2499,7 +2697,7 @@
         <v>84</v>
       </c>
       <c r="B63" t="s">
-        <v>209</v>
+        <v>275</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>10</v>
@@ -2522,7 +2720,7 @@
         <v>84</v>
       </c>
       <c r="B64" t="s">
-        <v>210</v>
+        <v>276</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>10</v>
@@ -2545,7 +2743,7 @@
         <v>84</v>
       </c>
       <c r="B65" t="s">
-        <v>211</v>
+        <v>277</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>10</v>
@@ -2568,7 +2766,7 @@
         <v>84</v>
       </c>
       <c r="B66" t="s">
-        <v>212</v>
+        <v>278</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>10</v>
@@ -2591,7 +2789,7 @@
         <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>213</v>
+        <v>279</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>10</v>

</xml_diff>